<commit_message>
Beaucoup de changement, UI paufiné, algo amélioré + intégration des intérims + création fichier excel
</commit_message>
<xml_diff>
--- a/Matrice de polyvalence.xlsx
+++ b/Matrice de polyvalence.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="175">
   <si>
     <t xml:space="preserve">(3) B 1604</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t xml:space="preserve">WEHRLEN Patrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VINCENT (Int.)</t>
   </si>
   <si>
     <t xml:space="preserve">0 = ne connait pas le poste, 1 = remplaçant occasionnel (dépannage), 2 =  remplaçant ponctuel à fréquent, 3 =  remplaçant très fréquent ou poste attitré, 4 = poste type lorsque tout le personnel est présent</t>
@@ -915,12 +918,8 @@
   </sheetPr>
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AC1" activeCellId="0" sqref="AC1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH15" activeCellId="0" sqref="AH15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R37" activeCellId="0" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5585,7 +5584,9 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B36" s="4" t="n">
         <v>0</v>
       </c>
@@ -5635,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="R36" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S36" s="4" t="n">
         <v>0</v>
@@ -5851,7 +5852,7 @@
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -5919,12 +5920,8 @@
   </sheetPr>
   <dimension ref="A1:AR43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y18" activeCellId="0" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6167,7 +6164,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>0</v>
@@ -6301,7 +6298,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>4</v>
@@ -6435,7 +6432,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>0</v>
@@ -6569,7 +6566,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>0</v>
@@ -6703,7 +6700,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>0</v>
@@ -6837,7 +6834,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>0</v>
@@ -6971,7 +6968,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>0</v>
@@ -7105,7 +7102,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>2</v>
@@ -7239,7 +7236,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>0</v>
@@ -7373,7 +7370,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>0</v>
@@ -7507,7 +7504,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>0</v>
@@ -7641,7 +7638,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>0</v>
@@ -7775,7 +7772,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>0</v>
@@ -7909,7 +7906,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>0</v>
@@ -8043,7 +8040,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>0</v>
@@ -8177,7 +8174,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>0</v>
@@ -8311,7 +8308,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>0</v>
@@ -8445,7 +8442,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>0</v>
@@ -8579,7 +8576,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>0</v>
@@ -8713,7 +8710,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>0</v>
@@ -8847,7 +8844,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>0</v>
@@ -8981,7 +8978,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>0</v>
@@ -9115,7 +9112,7 @@
     </row>
     <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>0</v>
@@ -9249,7 +9246,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>0</v>
@@ -9383,7 +9380,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>0</v>
@@ -9517,7 +9514,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>0</v>
@@ -9651,7 +9648,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>3</v>
@@ -9785,7 +9782,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>0</v>
@@ -9919,7 +9916,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B31" s="4" t="n">
         <v>0</v>
@@ -10053,7 +10050,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>0</v>
@@ -10187,7 +10184,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>0</v>
@@ -10321,7 +10318,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>1</v>
@@ -10455,7 +10452,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>0</v>
@@ -10589,7 +10586,7 @@
     </row>
     <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>0</v>
@@ -10723,7 +10720,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B37" s="4" t="n">
         <v>0</v>
@@ -11385,7 +11382,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -11436,12 +11433,8 @@
   </sheetPr>
   <dimension ref="A1:AR45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11684,7 +11677,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>0</v>
@@ -11818,7 +11811,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>0</v>
@@ -11952,7 +11945,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>2</v>
@@ -12086,7 +12079,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>0</v>
@@ -12220,7 +12213,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>2</v>
@@ -12354,7 +12347,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>0</v>
@@ -12488,7 +12481,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>1</v>
@@ -12622,7 +12615,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>0</v>
@@ -12756,7 +12749,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>0</v>
@@ -12890,7 +12883,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>0</v>
@@ -13024,7 +13017,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B13" s="8" t="n">
         <v>0</v>
@@ -13158,7 +13151,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B14" s="8" t="n">
         <v>2</v>
@@ -13292,7 +13285,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>2</v>
@@ -13426,7 +13419,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>0</v>
@@ -13560,7 +13553,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>0</v>
@@ -13694,7 +13687,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>0</v>
@@ -13828,7 +13821,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>3</v>
@@ -13962,7 +13955,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B20" s="8" t="n">
         <v>3</v>
@@ -14096,7 +14089,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B21" s="8" t="n">
         <v>0</v>
@@ -14230,7 +14223,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B22" s="8" t="n">
         <v>2</v>
@@ -14364,7 +14357,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B23" s="8" t="n">
         <v>0</v>
@@ -14498,7 +14491,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B24" s="8" t="n">
         <v>3</v>
@@ -14632,7 +14625,7 @@
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B25" s="8" t="n">
         <v>0</v>
@@ -14766,7 +14759,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B26" s="8" t="n">
         <v>0</v>
@@ -14900,7 +14893,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B27" s="8" t="n">
         <v>0</v>
@@ -15034,7 +15027,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B28" s="8" t="n">
         <v>0</v>
@@ -15168,7 +15161,7 @@
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B29" s="8" t="n">
         <v>0</v>
@@ -15302,7 +15295,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B30" s="8" t="n">
         <v>3</v>
@@ -15436,7 +15429,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B31" s="8" t="n">
         <v>0</v>
@@ -15570,7 +15563,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B32" s="8" t="n">
         <v>0</v>
@@ -15704,7 +15697,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B33" s="8" t="n">
         <v>0</v>
@@ -15838,7 +15831,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B34" s="8" t="n">
         <v>0</v>
@@ -15972,7 +15965,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B35" s="8" t="n">
         <v>3</v>
@@ -16106,7 +16099,7 @@
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B36" s="8" t="n">
         <v>3</v>
@@ -16240,7 +16233,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B37" s="8" t="n">
         <v>0</v>
@@ -16374,7 +16367,7 @@
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B38" s="8" t="n">
         <v>4</v>
@@ -16508,7 +16501,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B39" s="8" t="n">
         <v>3</v>
@@ -17170,7 +17163,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>